<commit_message>
Update for central vs distributed case study
</commit_message>
<xml_diff>
--- a/Projects/Central_vs_distributed/Data_files/CSV_data/GAMS_H2_price.xlsx
+++ b/Projects/Central_vs_distributed/Data_files/CSV_data/GAMS_H2_price.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeichman\Documents\gamsdir\projdir\RODeO\Projects\Central_vs_distributed\Data_files\CSV_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5155F6EC-69CD-493B-8CE0-8EA78C3FC939}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H2_price_hourly" sheetId="1" r:id="rId1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -870,12 +871,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8762"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>